<commit_message>
Added email notifications and structured invoice generation
</commit_message>
<xml_diff>
--- a/bookings.xlsx
+++ b/bookings.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,98 +465,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Girish Ramsing Pardeshi</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>7030663155</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>📱 Screen Replacement</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-07-07</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>02:38 PM</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-07-07 14:39:35</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Girish Ramsing Pardeshi</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>7030663155</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>🔄 Software Update</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2025-07-07</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>02:40 PM</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2025-07-07 14:42:08</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Girish Ramsing Pardeshi</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>7030663155</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>📱 Screen Replacement</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2025-07-07</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>07:00 PM</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2025-07-07 14:54:15</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>